<commit_message>
last version who workssssss
</commit_message>
<xml_diff>
--- a/Inventory_formated.xlsx
+++ b/Inventory_formated.xlsx
@@ -16,9 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t xml:space="preserve">Layer number</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+  <si>
+    <t xml:space="preserve">finishing type</t>
   </si>
   <si>
     <t>Electricity</t>
@@ -75,10 +75,16 @@
     <t>Water</t>
   </si>
   <si>
-    <t xml:space="preserve">Pad number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surface area per pad</t>
+    <t xml:space="preserve">Pad surface</t>
+  </si>
+  <si>
+    <t>Ni/Gold</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Silver</t>
   </si>
 </sst>
 </file>
@@ -113,10 +119,13 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="11" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -627,7 +636,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -698,174 +707,162 @@
       <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>17.975711333333333</v>
+      </c>
+      <c r="C2">
+        <v>1.5631053333333333</v>
+      </c>
+      <c r="D2">
+        <v>49.181150000000002</v>
+      </c>
+      <c r="E2" s="2">
+        <v>9.9999999999999998e-13</v>
       </c>
       <c r="F2">
-        <v>0.61499999999999999</v>
-      </c>
-      <c r="H2">
-        <v>0.31</v>
+        <v>0.14086158293750001</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2">
+        <v>0.50999118206250005</v>
+      </c>
+      <c r="J2">
+        <v>0.072267098375000005</v>
       </c>
       <c r="K2">
-        <v>1.8899999999999999</v>
+        <v>0.12910734706249999</v>
       </c>
       <c r="L2">
-        <v>0.00015474</v>
+        <v>0.00077280000000000014</v>
+      </c>
+      <c r="M2">
+        <v>0.017814</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0.023105000000000001</v>
       </c>
       <c r="P2">
-        <v>0.0080000000000000002</v>
+        <v>0.76807734124999993</v>
+      </c>
+      <c r="Q2">
+        <v>0.28661667943750002</v>
       </c>
       <c r="R2" s="1">
-        <v>0.069000000000000006</v>
-      </c>
-      <c r="S2" s="1"/>
+        <v>0.02265</v>
+      </c>
+      <c r="S2" s="1">
+        <v>4.443692693750001</v>
+      </c>
+      <c r="T2">
+        <v>0.40000000000000002</v>
+      </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="L3">
-        <v>0.00015474</v>
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="3">
+        <v>17.975711333333333</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1.5631053333333333</v>
+      </c>
+      <c r="D3" s="3">
+        <v>49.181150000000002</v>
+      </c>
+      <c r="E3" s="2">
+        <v>9.9999999999999998e-13</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.14086158293750001</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0.50999118206250005</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.072267098375000005</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0.12910734706249999</v>
+      </c>
+      <c r="L3" s="3">
+        <v>0</v>
+      </c>
+      <c r="M3" s="3">
+        <v>0</v>
+      </c>
+      <c r="N3" s="3">
+        <v>0.0012588</v>
+      </c>
+      <c r="O3" s="3">
+        <v>0.023105000000000001</v>
+      </c>
+      <c r="P3" s="3">
+        <v>0.76807734124999993</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>0.28661667943750002</v>
+      </c>
+      <c r="R3" s="3">
+        <v>0.02265</v>
+      </c>
+      <c r="S3" s="3">
+        <v>4.443692693750001</v>
+      </c>
+      <c r="T3" s="3">
+        <v>0.40000000000000002</v>
       </c>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4">
-        <v>4</v>
-      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>107.854268</v>
-      </c>
-      <c r="C5">
-        <v>9.3786319999999996</v>
-      </c>
-      <c r="D5">
-        <v>295.08690000000001</v>
-      </c>
-      <c r="E5" s="2">
-        <v>9.9999999999999998e-13</v>
-      </c>
-      <c r="F5">
-        <v>0.49313249999999997</v>
-      </c>
-      <c r="G5">
-        <v>0.51295000000000002</v>
-      </c>
-      <c r="H5">
-        <v>0.21329999999999999</v>
-      </c>
-      <c r="I5">
-        <v>3.7035999999999998</v>
-      </c>
-      <c r="J5">
-        <v>0.4803</v>
-      </c>
-      <c r="K5">
-        <v>0.23369999999999999</v>
-      </c>
-      <c r="L5">
-        <v>0.00015474</v>
-      </c>
-      <c r="M5">
-        <v>0.00076999999999999996</v>
-      </c>
-      <c r="N5">
-        <v>0.00051473999999999997</v>
-      </c>
-      <c r="O5">
-        <v>0.13863</v>
-      </c>
-      <c r="P5">
-        <v>1.8913</v>
-      </c>
-      <c r="Q5">
-        <v>0.31690000000000002</v>
-      </c>
-      <c r="R5">
-        <v>0.13589999999999999</v>
-      </c>
-      <c r="S5">
-        <v>6.5057</v>
-      </c>
+      <c r="E5" s="2"/>
     </row>
-    <row r="6" ht="14.25">
-      <c r="A6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" ht="14.25">
-      <c r="A7">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>130.1018</v>
-      </c>
-      <c r="C7">
-        <v>11.3132</v>
-      </c>
-      <c r="F7">
-        <v>1.7606528269999999</v>
-      </c>
-      <c r="I7">
-        <v>4.4562589130000001</v>
-      </c>
-      <c r="J7">
-        <v>0.67597357400000002</v>
-      </c>
-      <c r="K7">
-        <v>1.832017553</v>
-      </c>
-      <c r="M7">
-        <v>0.25618106800000001</v>
-      </c>
-      <c r="P7">
-        <v>10.39793746</v>
-      </c>
-      <c r="Q7">
-        <v>4.2689668709999999</v>
-      </c>
-      <c r="S7">
-        <v>1137.7453310000001</v>
-      </c>
-    </row>
-    <row r="8" ht="14.25">
-      <c r="A8">
-        <v>12</v>
-      </c>
-      <c r="F8">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" ht="14.25">
-      <c r="A9">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" ht="14.25">
-      <c r="A10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" ht="14.25">
-      <c r="A11">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" ht="14.25">
-      <c r="A12">
-        <v>20</v>
-      </c>
-    </row>
+    <row r="6" ht="14.25"/>
+    <row r="7" ht="14.25"/>
+    <row r="8" ht="14.25"/>
+    <row r="9" ht="14.25"/>
+    <row r="10" ht="14.25"/>
+    <row r="11" ht="14.25"/>
+    <row r="12" ht="14.25"/>
     <row r="13" ht="14.25"/>
     <row r="14" ht="14.25"/>
     <row r="15" ht="14.25"/>

</xml_diff>